<commit_message>
Sorting files by folders, add Gigachat and YandexGPT test
</commit_message>
<xml_diff>
--- a/application/output.xlsx
+++ b/application/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2971,81 +2971,6 @@
         </is>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="inlineStr"/>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>((учитель</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>Учитель (педагог)</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr"/>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>собака</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>Рабочий</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr"/>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>иррап</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>Рабочий</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr"/>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>teacher</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>Рабочий</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr"/>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>о</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>Рабочий</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>